<commit_message>
Classificação de relevância de tweets
</commit_message>
<xml_diff>
--- a/PlayStation 5.xlsx
+++ b/PlayStation 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/rafaelpp3_al_insper_edu_br/Documents/Ciencia dos Dados/Projeto1_CDados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Insper\Ciência dos Dados\Projeto1_CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{82817119-2F61-41C9-AEBF-87977263B779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35D2D4E0-6A76-4C4D-B3F6-08C40A25819B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B567805-4AE9-492F-8076-2DA47BEE2F97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2396,7 +2396,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2413,7 +2413,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2735,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="A301" sqref="A301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3948,755 +3948,1208 @@
       <c r="A151" t="s">
         <v>149</v>
       </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>150</v>
       </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>151</v>
       </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>152</v>
       </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>153</v>
       </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>154</v>
       </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>155</v>
       </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>156</v>
       </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>157</v>
       </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>299</v>
+      </c>
+      <c r="B301">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Classificação de tweets de teste
</commit_message>
<xml_diff>
--- a/PlayStation 5.xlsx
+++ b/PlayStation 5.xlsx
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Insper\Ciência dos Dados\Projeto1_CDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B567805-4AE9-492F-8076-2DA47BEE2F97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD113E-C85A-434E-BFEF-505C1430F1ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="503">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2735,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="A301" sqref="A301"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5163,1015 +5174,1628 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="255.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>500</v>
+      </c>
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6179,5 +6803,6 @@
     <hyperlink ref="A31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>